<commit_message>
adding invalid login test case
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B38\Workspace\b38april7\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0B5522-94F2-4EEB-98ED-EADB036AC152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B279EC-F9D4-4453-85B3-7FAAB11B505F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="1485" windowWidth="5385" windowHeight="7365" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test1" sheetId="1" r:id="rId1"/>
+    <sheet name="testValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="test2" sheetId="2" r:id="rId2"/>
     <sheet name="test3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>UN</t>
   </si>
@@ -35,24 +35,9 @@
     <t>PW</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>manager</t>
   </si>
   <si>
-    <t>bhanu</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>akshara</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -68,16 +53,28 @@
     <t>A3</t>
   </si>
   <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
     <t>B3</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>A4</t>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>E-Title</t>
+  </si>
+  <si>
+    <t>actiTIME - Enter Time-Track</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
   </si>
 </sst>
 </file>
@@ -395,10 +392,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC573F-2E18-46C4-84FD-8E9A157E5650}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,26 +450,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -440,58 +485,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AC573F-2E18-46C4-84FD-8E9A157E5650}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB86C3DB-1922-421A-94B6-D5F9DCA2F927}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -499,34 +497,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>